<commit_message>
did i fix it now, i believe so
</commit_message>
<xml_diff>
--- a/Data_files/Part_2/Rotterdam_car_adjacency_peri.xlsx
+++ b/Data_files/Part_2/Rotterdam_car_adjacency_peri.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimEW\PycharmProjects\Design_in_Network_group_8\Data_files\Part_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F580ECD9-AD43-48F9-9833-A6B09AC36BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B348DB3D-584B-4AE5-A714-D263B820B5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -756,7 +756,7 @@
   <dimension ref="A1:U39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="R26" sqref="R26"/>
+      <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1612,7 +1612,7 @@
         <v>1</v>
       </c>
       <c r="S13" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T13" s="14">
         <v>0</v>
@@ -1737,7 +1737,7 @@
         <v>0</v>
       </c>
       <c r="Q15" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R15" s="3">
         <v>0</v>
@@ -2000,21 +2000,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000967D3B9FC1DD84EB00B55E5790AB85E" ma:contentTypeVersion="4" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="92ec66a21d0d7142cf1fb1ae8fa08641">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6ba023f1-a19b-4eec-904c-052d1f1cb5e0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62a86672aac255264bf3f3decc56659c" ns2:_="">
     <xsd:import namespace="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
@@ -2158,10 +2143,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4089522E-0C82-47E8-A49E-84CDA0FE73C2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47226C14-663C-468E-81A1-C92460C7FBF2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2183,19 +2193,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47226C14-663C-468E-81A1-C92460C7FBF2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4089522E-0C82-47E8-A49E-84CDA0FE73C2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>